<commit_message>
Add missing REGLD to POP2
</commit_message>
<xml_diff>
--- a/Microcode Generator.xlsx
+++ b/Microcode Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Can\FÖDEVLER\CSE4117\HW1\cse4117-hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F0E95-BD69-46EC-A455-4D30B3776B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911733CC-F1D9-417D-AFA9-5325D66F3B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
@@ -2192,7 +2192,9 @@
         <v>1</v>
       </c>
       <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
+      <c r="T28" s="19">
+        <v>1</v>
+      </c>
       <c r="U28" s="19"/>
       <c r="V28" s="19">
         <v>1</v>
@@ -2204,11 +2206,11 @@
       </c>
       <c r="Z28" s="19" t="str" cm="1">
         <f t="array" ref="Z28">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E28:X28),0,1),DEC2BIN(Y28,5))</f>
-        <v>0000000000000000100010000000</v>
+        <v>0000000000000000101010000000</v>
       </c>
       <c r="AA28" s="19" t="str">
         <f>_xlfn.CONCAT(BIN2HEX(LEFT(Z28,8),2),BIN2HEX(MID(Z28,9,8),2),BIN2HEX(MID(Z28,17,8),2),BIN2HEX(RIGHT(Z28,4)))</f>
-        <v>0000880</v>
+        <v>0000A80</v>
       </c>
       <c r="AB28" s="18"/>
       <c r="AC28" s="18"/>
@@ -3164,16 +3166,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:R8"/>
+    <mergeCell ref="C3:R3"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="G15:R15"/>
     <mergeCell ref="G22:O22"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:R8"/>
-    <mergeCell ref="C3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Make it so Timer keeps its interrupt high until it's read.
</commit_message>
<xml_diff>
--- a/Microcode Generator.xlsx
+++ b/Microcode Generator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Can\FÖDEVLER\CSE4117\HW1\cse4117-hw1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan\DÖDEVLER\CSE4117\cse4117-hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911733CC-F1D9-417D-AFA9-5325D66F3B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D036167-36E5-4ACC-A0E4-0435995AF8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
   <sheets>
     <sheet name="microcode" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
   <dimension ref="C1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11:AA32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,16 +3166,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:R15"/>
+    <mergeCell ref="G22:O22"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:R8"/>
     <mergeCell ref="C3:R3"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:R15"/>
-    <mergeCell ref="G22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Interrupt routine can be entered.
Made changes to microcode. Added SLI and CLI to assembler. IRET is not added yet.
Added sample program with example ISR which does an infinite loop.
</commit_message>
<xml_diff>
--- a/Microcode Generator.xlsx
+++ b/Microcode Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan\DÖDEVLER\CSE4117\cse4117-hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D036167-36E5-4ACC-A0E4-0435995AF8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E022A7-0778-48C4-A89D-A1C1637AFA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
   <sheets>
     <sheet name="microcode" sheetId="1" r:id="rId1"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
   <dimension ref="C1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2048,9 @@
         <v>15</v>
       </c>
       <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="19">
+        <v>1</v>
+      </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
@@ -2084,11 +2086,11 @@
       </c>
       <c r="Z26" s="19" t="str" cm="1">
         <f t="array" ref="Z26">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E26:X26),0,1),DEC2BIN(Y26,5))</f>
-        <v>0000000000011010101010010001</v>
+        <v>0000100000011010101010010001</v>
       </c>
       <c r="AA26" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>001AA91</v>
+        <v>081AA91</v>
       </c>
       <c r="AB26" s="10"/>
       <c r="AC26" s="10"/>
@@ -2116,9 +2118,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="19"/>
-      <c r="F27" s="19">
-        <v>1</v>
-      </c>
+      <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
@@ -2144,11 +2144,11 @@
       </c>
       <c r="Z27" s="19" t="str" cm="1">
         <f t="array" ref="Z27">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E27:X27),0,1),DEC2BIN(Y27,5))</f>
-        <v>0000100000000000100000000000</v>
+        <v>0000000000000000100000000000</v>
       </c>
       <c r="AA27" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0800800</v>
+        <v>0000800</v>
       </c>
       <c r="AB27" s="10"/>
       <c r="AC27" s="10"/>
@@ -2315,7 +2315,9 @@
       </c>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="O30" s="19">
+        <v>1</v>
+      </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
       <c r="R30" s="19">
@@ -2330,15 +2332,15 @@
       </c>
       <c r="X30" s="19"/>
       <c r="Y30" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z30" s="19" t="str" cm="1">
         <f t="array" ref="Z30">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E30:X30),0,1),DEC2BIN(Y30,5))</f>
-        <v>0000000100100000100001010011</v>
+        <v>0000000100100100100001010100</v>
       </c>
       <c r="AA30" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0120853</v>
+        <v>0124854</v>
       </c>
       <c r="AB30" s="9"/>
       <c r="AC30" s="9"/>
@@ -2396,15 +2398,15 @@
       </c>
       <c r="X31" s="19"/>
       <c r="Y31" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Z31" s="19" t="str" cm="1">
         <f t="array" ref="Z31">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E31:X31),0,1),DEC2BIN(Y31,5))</f>
-        <v>0000011001000000100001010100</v>
+        <v>0000011001000000100001010101</v>
       </c>
       <c r="AA31" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0640854</v>
+        <v>0640855</v>
       </c>
       <c r="AB31" s="9"/>
       <c r="AC31" s="9"/>
@@ -3166,16 +3168,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:R8"/>
+    <mergeCell ref="C3:R3"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="G15:R15"/>
     <mergeCell ref="G22:O22"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:R8"/>
-    <mergeCell ref="C3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Interrupt masking is working. Useless signals removed from SLI and CLI.
</commit_message>
<xml_diff>
--- a/Microcode Generator.xlsx
+++ b/Microcode Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan\DÖDEVLER\CSE4117\cse4117-hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E022A7-0778-48C4-A89D-A1C1637AFA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4418D05-17BA-4109-9959-FE1FBE0A7859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
   <dimension ref="C1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A2972" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA32" sqref="AA11:AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,17 +1874,11 @@
       <c r="O23" s="19"/>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
-      <c r="R23" s="19">
-        <v>1</v>
-      </c>
+      <c r="R23" s="19"/>
       <c r="S23" s="19"/>
-      <c r="T23" s="19">
-        <v>1</v>
-      </c>
+      <c r="T23" s="19"/>
       <c r="U23" s="19"/>
-      <c r="V23" s="19">
-        <v>1</v>
-      </c>
+      <c r="V23" s="19"/>
       <c r="W23" s="19"/>
       <c r="X23" s="19"/>
       <c r="Y23" s="8">
@@ -1892,11 +1886,11 @@
       </c>
       <c r="Z23" s="19" t="str" cm="1">
         <f t="array" ref="Z23">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E23:X23),0,1),DEC2BIN(Y23,5))</f>
-        <v>0000000010000000101010000000</v>
+        <v>0000000010000000000000000000</v>
       </c>
       <c r="AA23" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0080A80</v>
+        <v>0080000</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
@@ -1933,24 +1927,16 @@
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="19">
-        <v>1</v>
-      </c>
+      <c r="M24" s="19"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
-      <c r="P24" s="19">
-        <v>1</v>
-      </c>
+      <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
-      <c r="R24" s="19">
-        <v>1</v>
-      </c>
+      <c r="R24" s="19"/>
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
       <c r="U24" s="19"/>
-      <c r="V24" s="19">
-        <v>1</v>
-      </c>
+      <c r="V24" s="19"/>
       <c r="W24" s="19"/>
       <c r="X24" s="19"/>
       <c r="Y24" s="8">
@@ -1958,11 +1944,11 @@
       </c>
       <c r="Z24" s="19" t="str" cm="1">
         <f t="array" ref="Z24">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E24:X24),0,1),DEC2BIN(Y24,5))</f>
-        <v>0000000100010010100010000000</v>
+        <v>0000000100000000000000000000</v>
       </c>
       <c r="AA24" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0112880</v>
+        <v>0100000</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="10"/>
@@ -3168,16 +3154,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:R15"/>
+    <mergeCell ref="G22:O22"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:R8"/>
     <mergeCell ref="C3:R3"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:R15"/>
-    <mergeCell ref="G22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed PCLD signal from CALL.
</commit_message>
<xml_diff>
--- a/Microcode Generator.xlsx
+++ b/Microcode Generator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan\DÖDEVLER\CSE4117\cse4117-hw1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Can\FÖDEVLER\CSE4117\HW1\cse4117-hw1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF00AD4-92E9-4325-809C-A8418CCB5B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AFC06C-A98F-45CA-A7ED-23E4F096A4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
   <sheets>
     <sheet name="microcode" sheetId="1" r:id="rId1"/>
@@ -351,8 +351,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,8 +372,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,7 +393,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -692,8 +692,8 @@
   <dimension ref="C1:AQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2:AA23"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,9 +1414,7 @@
       <c r="O12" s="19">
         <v>1</v>
       </c>
-      <c r="P12" s="19">
-        <v>1</v>
-      </c>
+      <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19">
         <v>1</v>
@@ -1430,15 +1428,15 @@
       </c>
       <c r="X12" s="19"/>
       <c r="Y12" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z12" s="19" t="str" cm="1">
         <f t="array" ref="Z12">_xlfn.CONCAT(REPT(0,3),IF(ISBLANK(E12:X12),0,1),DEC2BIN(Y12,5))</f>
-        <v>0000000000100110100001000000</v>
+        <v>0000000000100100100001000101</v>
       </c>
       <c r="AA12" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>0026840</v>
+        <v>0024845</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
@@ -1661,7 +1659,7 @@
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="29">
+      <c r="Y16" s="22">
         <v>15</v>
       </c>
       <c r="Z16" s="19" t="str" cm="1">
@@ -2167,24 +2165,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>

</xml_diff>